<commit_message>
Arranged xlsx for eLIMS
</commit_message>
<xml_diff>
--- a/CONFIG/lists.xlsx
+++ b/CONFIG/lists.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CF6P\Desktop\ECAR\OCR_ECAR\CONFIG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FDB1D7B-0C7C-42CE-AF44-23287383580A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51581D74-EFDA-4F43-BF96-CDF6784029BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -420,7 +420,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>